<commit_message>
Added Verification for Mingbo Inheritance document
</commit_message>
<xml_diff>
--- a/Project_Inheritance_Documentation/Branch_2_ Inheritance/David - Handover.xlsx
+++ b/Project_Inheritance_Documentation/Branch_2_ Inheritance/David - Handover.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f337a85aa8871bf9/Desktop/japanese_project/japanese-handwriting-analysis/Project_Inheritance_Documentation/Branch_2_ Inheritance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANU\Semester_3\Advanced_Computing_Project\Project_Repo\japanese-handwriting-analysis\Project_Inheritance_Documentation\Branch_2_ Inheritance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{38B3E9DC-5AA2-4C47-A3C4-4A27063DB773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5554EC50-53F7-4E27-9521-5891D8DC88F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD0EA61-0520-44EE-9B03-8906C1D80AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>How to Use It</t>
   </si>
@@ -314,6 +312,15 @@
   </si>
   <si>
     <t>Mingbo</t>
+  </si>
+  <si>
+    <t>Yes, he explained somebit of it to me</t>
+  </si>
+  <si>
+    <t>Know that where the code is  and how to run on my system, but still need to dive deep into its concept to get it fully understood.</t>
+  </si>
+  <si>
+    <t>Can explain it to the new members next semester and will try to understand maximum of it during summer vacation</t>
   </si>
 </sst>
 </file>
@@ -481,6 +488,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -499,7 +507,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -836,43 +843,43 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.06640625" customWidth="1"/>
-    <col min="5" max="5" width="27.59765625" customWidth="1"/>
-    <col min="6" max="6" width="91.06640625" customWidth="1"/>
-    <col min="7" max="7" width="21.265625" customWidth="1"/>
-    <col min="8" max="8" width="47.59765625" customWidth="1"/>
-    <col min="9" max="14" width="21.46484375" customWidth="1"/>
+    <col min="1" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="91" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="14" width="21.42578125" customWidth="1"/>
     <col min="15" max="15" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="11" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="12"/>
-      <c r="O1" s="13"/>
-    </row>
-    <row r="2" spans="1:15" ht="28.5">
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
+    </row>
+    <row r="2" spans="1:15" ht="30">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -950,7 +957,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="239" customHeight="1">
+    <row r="4" spans="1:15" ht="239.1" customHeight="1">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -978,7 +985,7 @@
       <c r="I4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="8">
         <v>45570</v>
       </c>
       <c r="K4" s="6" t="s">
@@ -987,11 +994,17 @@
       <c r="L4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" ht="187.05" customHeight="1">
+      <c r="M4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="187.15" customHeight="1">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1019,7 +1032,7 @@
       <c r="I5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="8">
         <v>45570</v>
       </c>
       <c r="K5" s="6" t="s">
@@ -1028,11 +1041,17 @@
       <c r="L5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" ht="270.75">
+      <c r="M5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="330">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -1060,7 +1079,7 @@
       <c r="I6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="8">
         <v>45570</v>
       </c>
       <c r="K6" s="6" t="s">
@@ -1069,9 +1088,15 @@
       <c r="L6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="256.5" customHeight="1">
       <c r="A7" s="5">
@@ -1101,7 +1126,7 @@
       <c r="I7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="8">
         <v>45570</v>
       </c>
       <c r="K7" s="6" t="s">
@@ -1110,11 +1135,17 @@
       <c r="L7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" ht="42.75">
+      <c r="M7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="90">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -1142,16 +1173,22 @@
       <c r="I8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="8">
         <v>45570</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="M8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="5"/>

</xml_diff>